<commit_message>
XLSX Bon de travail almost done
</commit_message>
<xml_diff>
--- a/Bon_de_travail.xlsx
+++ b/Bon_de_travail.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Numéro de requête</t>
   </si>
@@ -22,6 +22,9 @@
     <t>Numéro civique</t>
   </si>
   <si>
+    <t>Rue</t>
+  </si>
+  <si>
     <t>Pièce</t>
   </si>
   <si>
@@ -31,6 +34,9 @@
     <t>BAC BRUN - 45</t>
   </si>
   <si>
+    <t>BAC BRUN - 80</t>
+  </si>
+  <si>
     <t>BAC BRUN - 120</t>
   </si>
   <si>
@@ -53,6 +59,9 @@
   </si>
   <si>
     <t>corps</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
   <si>
     <t>79</t>
@@ -103,8 +112,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,83 +411,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="20.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="12" width="15.7109375" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2">
+    <row r="2" spans="1:13">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3">
+    <row r="3" spans="1:13">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4">
+    <row r="4" spans="1:13">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Styling && python fixes
</commit_message>
<xml_diff>
--- a/Bon_de_travail.xlsx
+++ b/Bon_de_travail.xlsx
@@ -55,10 +55,10 @@
     <t>141</t>
   </si>
   <si>
-    <t>Rue Amherst</t>
-  </si>
-  <si>
-    <t>corps</t>
+    <t>RUE AMHERST</t>
+  </si>
+  <si>
+    <t>CORPS</t>
   </si>
   <si>
     <t>1</t>
@@ -67,16 +67,16 @@
     <t>79</t>
   </si>
   <si>
-    <t>Chemin Fraser</t>
-  </si>
-  <si>
-    <t>couvercle</t>
+    <t>CHEMIN FRASER</t>
+  </si>
+  <si>
+    <t>COUVERCLE</t>
   </si>
   <si>
     <t>321</t>
   </si>
   <si>
-    <t>Boulevard Saint-Raymond</t>
+    <t>BOULEVARD SAINT-RAYMOND</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
@@ -482,7 +482,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>16</v>
@@ -499,7 +499,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>19</v>

</xml_diff>